<commit_message>
created new optimize_test_continuous.py file
It solves the same problem as optimize_with_activation but has less binary variables
</commit_message>
<xml_diff>
--- a/Variables_for_grid_optimization_completed.xlsx
+++ b/Variables_for_grid_optimization_completed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stanislashildebrandt/Desktop/local microgrid optimization/Microgrid_optimization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stanislashildebrandt/Documents/GitHub/Microgrid_optimization_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F92772C-6762-8B46-9444-407D1C57A349}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCB9B64-C1FF-4E46-A992-A9FBFD634B36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BDABE487-912E-834B-9FFB-2F135B5C8AD3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="158">
   <si>
     <t>P[k]</t>
   </si>
@@ -499,6 +499,12 @@
   </si>
   <si>
     <t>CAPBAT * CAPEXVARIABLEBAT is in the objective function</t>
+  </si>
+  <si>
+    <t>flow(pv,bat) &lt;= CCHARGEMAXBAT * CAPBAT</t>
+  </si>
+  <si>
+    <t>flow(bat,cons) &lt;= CDISCHARGEMAXBAT * CAPBAT</t>
   </si>
 </sst>
 </file>
@@ -884,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2E8697-2373-5049-9EDF-FA626E8CB93D}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1150,6 +1156,9 @@
       <c r="F13" s="3">
         <v>1</v>
       </c>
+      <c r="G13" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1169,6 +1178,9 @@
       </c>
       <c r="F14" s="3">
         <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated cost function, modified excel
</commit_message>
<xml_diff>
--- a/Variables_for_grid_optimization_completed.xlsx
+++ b/Variables_for_grid_optimization_completed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stanislashildebrandt/Documents/GitHub/Microgrid_optimization_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCB9B64-C1FF-4E46-A992-A9FBFD634B36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBD14E7-DF88-AD41-A772-C4EBF6593BD7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BDABE487-912E-834B-9FFB-2F135B5C8AD3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{BDABE487-912E-834B-9FFB-2F135B5C8AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="169">
   <si>
     <t>P[k]</t>
   </si>
@@ -243,9 +243,6 @@
     <t>CAPEXVARIABLESOLAR</t>
   </si>
   <si>
-    <t>OPEXFFIXEDSOLAR</t>
-  </si>
-  <si>
     <t>OPEXVARIABLESOLAR</t>
   </si>
   <si>
@@ -444,9 +441,6 @@
     <t>number of super source PV nodes</t>
   </si>
   <si>
-    <t>in objective function non_zero_pv * CAPEXFIXEDSOLAR</t>
-  </si>
-  <si>
     <t>pv_activation_vars</t>
   </si>
   <si>
@@ -498,13 +492,52 @@
     <t>supersupersourcePV</t>
   </si>
   <si>
-    <t>CAPBAT * CAPEXVARIABLEBAT is in the objective function</t>
-  </si>
-  <si>
     <t>flow(pv,bat) &lt;= CCHARGEMAXBAT * CAPBAT</t>
   </si>
   <si>
     <t>flow(bat,cons) &lt;= CDISCHARGEMAXBAT * CAPBAT</t>
+  </si>
+  <si>
+    <t>OPEXFIXEDSOLAR</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>will be used later in added nodes between pv and bat</t>
+  </si>
+  <si>
+    <t>will be used later in added nodes between bat and cons</t>
+  </si>
+  <si>
+    <t>cost function</t>
+  </si>
+  <si>
+    <t>decision variable</t>
+  </si>
+  <si>
+    <t>used as lower bound in cons supersink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost function </t>
+  </si>
+  <si>
+    <t>cost function  prated_solar * (CAPEXVARIABLESOLAR / LIFETIMESOLAR + OPEXVARIABLESOLAR)</t>
+  </si>
+  <si>
+    <t>cost function  non_zero_pv * ((CAPEXFIXEDSOLAR)/(LIFETIMESOLAR)</t>
+  </si>
+  <si>
+    <t>cost function cap_bat * (CAPEXVARIABLEBAT / LIFETIMEBAT + OPEXVARIABLEBAT)</t>
+  </si>
+  <si>
+    <t>cost function  cap_bat * (CAPEXVARIABLEBAT / LIFETIMEBAT + OPEXVARIABLEBAT)</t>
+  </si>
+  <si>
+    <t>cost function  non_zero_bat * ((CAPEXFIXEDBAT)/(LIFETIMEBAT) + OPEXFIXEDBAT)</t>
+  </si>
+  <si>
+    <t>upper bound flow_vars[supsrcPV,PVi] &lt;= PNORMSOLAR[i] * prated_solar</t>
   </si>
 </sst>
 </file>
@@ -890,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2E8697-2373-5049-9EDF-FA626E8CB93D}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="86" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -923,10 +956,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -943,15 +976,18 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="G2" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -968,13 +1004,13 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4" s="3">
         <v>0.2</v>
       </c>
       <c r="G4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -991,10 +1027,13 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F5" s="3">
         <v>80</v>
+      </c>
+      <c r="G5" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1011,13 +1050,13 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F6" s="3">
         <v>0.05</v>
       </c>
       <c r="G6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1034,13 +1073,13 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="3">
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1057,13 +1096,13 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F8" s="3">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1080,15 +1119,18 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1105,13 +1147,13 @@
         <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1128,13 +1170,13 @@
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F12" s="3">
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1151,13 +1193,13 @@
         <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1174,13 +1216,13 @@
         <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1194,10 +1236,13 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F15" s="3">
         <v>0.95</v>
+      </c>
+      <c r="G15" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1211,10 +1256,13 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F16" s="3">
         <v>0.95</v>
+      </c>
+      <c r="G16" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1231,10 +1279,13 @@
         <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F17" s="3">
         <v>3700</v>
+      </c>
+      <c r="G17" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1251,13 +1302,13 @@
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F18" s="3">
         <v>470</v>
       </c>
       <c r="G18" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1274,10 +1325,13 @@
         <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19" s="3">
         <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1294,10 +1348,13 @@
         <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F20" s="3">
         <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1314,10 +1371,13 @@
         <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21" s="3">
         <v>10</v>
+      </c>
+      <c r="G21" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1334,10 +1394,13 @@
         <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="G22" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1354,15 +1417,18 @@
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="G23" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1379,13 +1445,13 @@
         <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F25" s="3">
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1402,13 +1468,13 @@
         <v>55</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F26" s="3">
         <v>25</v>
       </c>
       <c r="G26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1425,10 +1491,13 @@
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="G27" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1451,7 +1520,7 @@
         <v>10000</v>
       </c>
       <c r="G28" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1473,6 +1542,9 @@
       <c r="F29" s="3">
         <v>1200</v>
       </c>
+      <c r="G29" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -1488,10 +1560,13 @@
         <v>45</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>155</v>
       </c>
       <c r="F30" s="3">
         <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1499,7 +1574,7 @@
         <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -1508,10 +1583,13 @@
         <v>46</v>
       </c>
       <c r="E31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F31" s="3">
         <v>25</v>
+      </c>
+      <c r="G31" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1528,13 +1606,16 @@
         <v>48</v>
       </c>
       <c r="E32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F32" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -1548,18 +1629,21 @@
         <v>55</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="G33" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
         <v>22</v>
@@ -1568,62 +1652,65 @@
         <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="G34" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B36" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C36" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C37" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F39" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F39" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B40" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1632,54 +1719,54 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B44" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1688,12 +1775,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B45" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -1702,26 +1789,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B46" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B47" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1732,63 +1819,63 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B56" s="1"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature - added max power price in cost function
</commit_message>
<xml_diff>
--- a/Variables_for_grid_optimization_completed.xlsx
+++ b/Variables_for_grid_optimization_completed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stanislashildebrandt/Documents/GitHub/Microgrid_optimization_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBD14E7-DF88-AD41-A772-C4EBF6593BD7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DED19AA-BDA2-4346-A56A-2C8B450448C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{BDABE487-912E-834B-9FFB-2F135B5C8AD3}"/>
   </bookViews>
@@ -501,9 +501,6 @@
     <t>OPEXFIXEDSOLAR</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>will be used later in added nodes between pv and bat</t>
   </si>
   <si>
@@ -538,6 +535,9 @@
   </si>
   <si>
     <t>upper bound flow_vars[supsrcPV,PVi] &lt;= PNORMSOLAR[i] * prated_solar</t>
+  </si>
+  <si>
+    <t>multiplies max of consumption and added to the cost function</t>
   </si>
 </sst>
 </file>
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2E8697-2373-5049-9EDF-FA626E8CB93D}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="86" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="86" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -982,7 +982,7 @@
         <v>125</v>
       </c>
       <c r="G2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1033,7 +1033,7 @@
         <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1242,7 +1242,7 @@
         <v>0.95</v>
       </c>
       <c r="G15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1262,7 +1262,7 @@
         <v>0.95</v>
       </c>
       <c r="G16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1285,7 +1285,7 @@
         <v>3700</v>
       </c>
       <c r="G17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1308,7 +1308,7 @@
         <v>470</v>
       </c>
       <c r="G18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1331,7 +1331,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1354,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1377,7 +1377,7 @@
         <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1400,7 +1400,7 @@
         <v>126</v>
       </c>
       <c r="G22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1423,7 +1423,7 @@
         <v>126</v>
       </c>
       <c r="G23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1497,7 +1497,7 @@
         <v>125</v>
       </c>
       <c r="G27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1520,7 +1520,7 @@
         <v>10000</v>
       </c>
       <c r="G28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1543,7 +1543,7 @@
         <v>1200</v>
       </c>
       <c r="G29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1566,7 +1566,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1589,7 +1589,7 @@
         <v>25</v>
       </c>
       <c r="G31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1612,7 +1612,7 @@
         <v>25</v>
       </c>
       <c r="G32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1635,7 +1635,7 @@
         <v>126</v>
       </c>
       <c r="G33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1658,7 +1658,7 @@
         <v>126</v>
       </c>
       <c r="G34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added new parameters to excel
</commit_message>
<xml_diff>
--- a/Variables_for_grid_optimization_completed.xlsx
+++ b/Variables_for_grid_optimization_completed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stanislashildebrandt/Documents/GitHub/Microgrid_optimization_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DED19AA-BDA2-4346-A56A-2C8B450448C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF071C90-7F5B-CE42-B79A-22D5BD73630D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{BDABE487-912E-834B-9FFB-2F135B5C8AD3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BDABE487-912E-834B-9FFB-2F135B5C8AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="179">
   <si>
     <t>P[k]</t>
   </si>
@@ -387,12 +387,6 @@
     <t>"-PEXCHANGEDGRID" (?)</t>
   </si>
   <si>
-    <t>25 parameter variables</t>
-  </si>
-  <si>
-    <t>5 decision variables (counting PGENSOLAR)</t>
-  </si>
-  <si>
     <t>Super source</t>
   </si>
   <si>
@@ -538,6 +532,42 @@
   </si>
   <si>
     <t>multiplies max of consumption and added to the cost function</t>
+  </si>
+  <si>
+    <t>Electric Vehicle</t>
+  </si>
+  <si>
+    <t>Size of battery</t>
+  </si>
+  <si>
+    <t>CAP_BAT_EV</t>
+  </si>
+  <si>
+    <t>hourly presence of the car</t>
+  </si>
+  <si>
+    <t>HOURLY_PRESENCE_YEAR</t>
+  </si>
+  <si>
+    <t>vector of 0's and 1's</t>
+  </si>
+  <si>
+    <t>charging efficiency</t>
+  </si>
+  <si>
+    <t>ETA_CHARGE_EV</t>
+  </si>
+  <si>
+    <t>discharging efficiency</t>
+  </si>
+  <si>
+    <t>ETA_DISCHARGE_EV</t>
+  </si>
+  <si>
+    <t>minimum charge before leaving garage</t>
+  </si>
+  <si>
+    <t>MIN_LEAVING_CHARGE</t>
   </si>
 </sst>
 </file>
@@ -921,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2E8697-2373-5049-9EDF-FA626E8CB93D}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="86" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="86" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -956,10 +986,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -979,10 +1009,10 @@
         <v>88</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1010,7 +1040,7 @@
         <v>0.2</v>
       </c>
       <c r="G4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1033,7 +1063,7 @@
         <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1056,7 +1086,7 @@
         <v>0.05</v>
       </c>
       <c r="G6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1079,7 +1109,7 @@
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1102,7 +1132,7 @@
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1122,7 +1152,7 @@
         <v>89</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G9" t="s">
         <v>22</v>
@@ -1153,7 +1183,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1176,7 +1206,7 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1193,13 +1223,13 @@
         <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1222,7 +1252,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1235,6 +1265,9 @@
       <c r="C15" t="s">
         <v>3</v>
       </c>
+      <c r="D15" t="s">
+        <v>124</v>
+      </c>
       <c r="E15" t="s">
         <v>98</v>
       </c>
@@ -1242,7 +1275,7 @@
         <v>0.95</v>
       </c>
       <c r="G15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1255,6 +1288,9 @@
       <c r="C16" t="s">
         <v>3</v>
       </c>
+      <c r="D16" t="s">
+        <v>124</v>
+      </c>
       <c r="E16" t="s">
         <v>99</v>
       </c>
@@ -1262,7 +1298,7 @@
         <v>0.95</v>
       </c>
       <c r="G16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1285,7 +1321,7 @@
         <v>3700</v>
       </c>
       <c r="G17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1308,7 +1344,7 @@
         <v>470</v>
       </c>
       <c r="G18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1331,7 +1367,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1354,7 +1390,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1377,7 +1413,7 @@
         <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1397,10 +1433,10 @@
         <v>76</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1420,10 +1456,10 @@
         <v>90</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1451,7 +1487,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1474,7 +1510,7 @@
         <v>25</v>
       </c>
       <c r="G26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1494,10 +1530,10 @@
         <v>91</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G27" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1520,7 +1556,7 @@
         <v>10000</v>
       </c>
       <c r="G28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1543,7 +1579,7 @@
         <v>1200</v>
       </c>
       <c r="G29" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1560,13 +1596,13 @@
         <v>45</v>
       </c>
       <c r="E30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F30" s="3">
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1574,7 +1610,7 @@
         <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -1589,7 +1625,7 @@
         <v>25</v>
       </c>
       <c r="G31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1612,7 +1648,7 @@
         <v>25</v>
       </c>
       <c r="G32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1632,10 +1668,10 @@
         <v>73</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G33" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1655,18 +1691,18 @@
         <v>92</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C36" t="s">
         <v>22</v>
@@ -1674,208 +1710,103 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B37" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C37" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F38" t="s">
-        <v>118</v>
+      <c r="A38" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F39" t="s">
-        <v>119</v>
+      <c r="B39" t="s">
+        <v>168</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" t="s">
+        <v>169</v>
+      </c>
+      <c r="F39">
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>102</v>
-      </c>
       <c r="B40" t="s">
-        <v>141</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
+        <v>170</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" t="s">
+        <v>171</v>
+      </c>
+      <c r="F40" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>103</v>
-      </c>
       <c r="B41" t="s">
-        <v>142</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
+        <v>173</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>98</v>
+        <v>124</v>
+      </c>
+      <c r="E41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F41">
+        <v>0.95</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>104</v>
-      </c>
       <c r="B42" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>124</v>
+      </c>
+      <c r="E42" t="s">
+        <v>176</v>
+      </c>
+      <c r="F42">
+        <v>0.95</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>105</v>
-      </c>
       <c r="B43" t="s">
-        <v>144</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
+        <v>177</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>145</v>
-      </c>
-      <c r="B44" t="s">
-        <v>146</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>147</v>
-      </c>
-      <c r="B45" t="s">
-        <v>148</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>107</v>
-      </c>
-      <c r="B46" t="s">
-        <v>149</v>
-      </c>
-      <c r="C46" t="s">
-        <v>115</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>106</v>
-      </c>
-      <c r="B47" t="s">
-        <v>150</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>110</v>
-      </c>
-      <c r="B51" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>109</v>
-      </c>
-      <c r="B52" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B53" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>112</v>
-      </c>
-      <c r="B54" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>121</v>
-      </c>
-      <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>152</v>
+        <v>25</v>
+      </c>
+      <c r="E43" t="s">
+        <v>178</v>
+      </c>
+      <c r="F43">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -1886,14 +1817,207 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564B6298-8728-3449-98E7-4ED4EA8B4DA3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C7"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="4" width="19.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feature - added modified program where we run with various time reolutions
resolutions can be 1 hour, 1.5 hours, 2 hours, 3 hours
</commit_message>
<xml_diff>
--- a/Variables_for_grid_optimization_completed.xlsx
+++ b/Variables_for_grid_optimization_completed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stanislashildebrandt/Documents/GitHub/Microgrid_optimization_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D212C5-5D72-B647-9D85-335F3FA8B7B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4F5FDE-7096-4842-AD93-5920FDA3DCC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BDABE487-912E-834B-9FFB-2F135B5C8AD3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="183">
   <si>
     <t>P[k]</t>
   </si>
@@ -580,12 +580,6 @@
   </si>
   <si>
     <t>CDISCHARGE_MAX_EV</t>
-  </si>
-  <si>
-    <t>price of energy bought by recharging the car in the city</t>
-  </si>
-  <si>
-    <t>CENERGY_CITY</t>
   </si>
 </sst>
 </file>
@@ -969,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2E8697-2373-5049-9EDF-FA626E8CB93D}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="86" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1876,23 +1870,6 @@
       </c>
       <c r="F46">
         <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>183</v>
-      </c>
-      <c r="C47" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" t="s">
-        <v>184</v>
-      </c>
-      <c r="F47">
-        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>